<commit_message>
DistrictHeating 'smart heating' functionality
DistrictHeating controller with primary, secondary and backup heating systems functional, based on electricitySurpluss of Holon.
Not yet tuned.
</commit_message>
<xml_diff>
--- a/Base/APIOutputAgentData_300_gridConnections.xlsx
+++ b/Base/APIOutputAgentData_300_gridConnections.xlsx
@@ -746,7 +746,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -796,7 +796,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R4" t="inlineStr">
@@ -1411,7 +1411,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -1461,7 +1461,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R11" t="inlineStr">
@@ -1506,7 +1506,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -1556,7 +1556,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R12" t="inlineStr">
@@ -1601,7 +1601,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -1651,7 +1651,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R13" t="inlineStr">
@@ -2266,7 +2266,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
@@ -2631,12 +2631,12 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -2646,7 +2646,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -2696,7 +2696,7 @@
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R24" t="inlineStr">
@@ -2726,12 +2726,12 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>hol1</t>
+          <t>sup1</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
+          <t>root.pop_energySuppliers[0]</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -3296,12 +3296,12 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -3311,7 +3311,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -3361,7 +3361,7 @@
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R31" t="inlineStr">
@@ -3391,12 +3391,12 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -3406,7 +3406,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
@@ -3456,7 +3456,7 @@
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R32" t="inlineStr">
@@ -3486,12 +3486,12 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -3501,7 +3501,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -3551,7 +3551,7 @@
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R33" t="inlineStr">
@@ -4341,12 +4341,12 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -4356,7 +4356,7 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
@@ -4406,7 +4406,7 @@
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R42" t="inlineStr">
@@ -5006,12 +5006,12 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
@@ -5021,7 +5021,7 @@
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
@@ -5071,7 +5071,7 @@
       </c>
       <c r="Q49" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R49" t="inlineStr">
@@ -5101,12 +5101,12 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -5116,7 +5116,7 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
@@ -5166,7 +5166,7 @@
       </c>
       <c r="Q50" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R50" t="inlineStr">
@@ -5196,12 +5196,12 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
@@ -5211,7 +5211,7 @@
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H51" t="inlineStr">
@@ -5261,7 +5261,7 @@
       </c>
       <c r="Q51" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R51" t="inlineStr">
@@ -6051,12 +6051,12 @@
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -6066,7 +6066,7 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
@@ -6116,7 +6116,7 @@
       </c>
       <c r="Q60" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R60" t="inlineStr">
@@ -6716,12 +6716,12 @@
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -6731,7 +6731,7 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
@@ -6781,7 +6781,7 @@
       </c>
       <c r="Q67" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R67" t="inlineStr">
@@ -6811,12 +6811,12 @@
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
@@ -6826,7 +6826,7 @@
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H68" t="inlineStr">
@@ -6876,7 +6876,7 @@
       </c>
       <c r="Q68" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R68" t="inlineStr">
@@ -6906,12 +6906,12 @@
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
@@ -6921,7 +6921,7 @@
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
@@ -6971,7 +6971,7 @@
       </c>
       <c r="Q69" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R69" t="inlineStr">
@@ -7761,12 +7761,12 @@
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>sup2</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
@@ -7776,7 +7776,7 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
@@ -7826,7 +7826,7 @@
       </c>
       <c r="Q78" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R78" t="inlineStr">
@@ -8426,12 +8426,12 @@
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>sup2</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -8441,7 +8441,7 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
@@ -8491,7 +8491,7 @@
       </c>
       <c r="Q85" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R85" t="inlineStr">
@@ -8521,12 +8521,12 @@
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>sup2</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -8536,7 +8536,7 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
@@ -8586,7 +8586,7 @@
       </c>
       <c r="Q86" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R86" t="inlineStr">
@@ -8616,12 +8616,12 @@
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>sup2</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
@@ -8631,7 +8631,7 @@
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
@@ -8681,7 +8681,7 @@
       </c>
       <c r="Q87" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R87" t="inlineStr">
@@ -9471,12 +9471,12 @@
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>sup2</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
@@ -9486,7 +9486,7 @@
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
@@ -9536,7 +9536,7 @@
       </c>
       <c r="Q96" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R96" t="inlineStr">
@@ -10136,12 +10136,12 @@
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>sup2</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F103" t="inlineStr">
@@ -10151,7 +10151,7 @@
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H103" t="inlineStr">
@@ -10201,7 +10201,7 @@
       </c>
       <c r="Q103" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R103" t="inlineStr">
@@ -10231,12 +10231,12 @@
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>sup2</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F104" t="inlineStr">
@@ -10246,7 +10246,7 @@
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H104" t="inlineStr">
@@ -10296,7 +10296,7 @@
       </c>
       <c r="Q104" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R104" t="inlineStr">
@@ -10516,12 +10516,12 @@
       </c>
       <c r="D107" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
@@ -10531,7 +10531,7 @@
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H107" t="inlineStr">
@@ -10581,7 +10581,7 @@
       </c>
       <c r="Q107" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R107" t="inlineStr">
@@ -11181,12 +11181,12 @@
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F114" t="inlineStr">
@@ -11196,7 +11196,7 @@
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H114" t="inlineStr">
@@ -11246,7 +11246,7 @@
       </c>
       <c r="Q114" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R114" t="inlineStr">
@@ -11276,12 +11276,12 @@
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
@@ -11291,7 +11291,7 @@
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H115" t="inlineStr">
@@ -11341,7 +11341,7 @@
       </c>
       <c r="Q115" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R115" t="inlineStr">
@@ -11371,12 +11371,12 @@
       </c>
       <c r="D116" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
@@ -11386,7 +11386,7 @@
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H116" t="inlineStr">
@@ -11436,7 +11436,7 @@
       </c>
       <c r="Q116" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R116" t="inlineStr">
@@ -12226,12 +12226,12 @@
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
@@ -12241,7 +12241,7 @@
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H125" t="inlineStr">
@@ -12291,7 +12291,7 @@
       </c>
       <c r="Q125" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R125" t="inlineStr">
@@ -12891,12 +12891,12 @@
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
@@ -12906,7 +12906,7 @@
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H132" t="inlineStr">
@@ -12956,7 +12956,7 @@
       </c>
       <c r="Q132" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R132" t="inlineStr">
@@ -12986,12 +12986,12 @@
       </c>
       <c r="D133" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
@@ -13001,7 +13001,7 @@
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H133" t="inlineStr">
@@ -13051,7 +13051,7 @@
       </c>
       <c r="Q133" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R133" t="inlineStr">
@@ -13081,12 +13081,12 @@
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
@@ -13096,7 +13096,7 @@
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H134" t="inlineStr">
@@ -13146,7 +13146,7 @@
       </c>
       <c r="Q134" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R134" t="inlineStr">
@@ -13936,12 +13936,12 @@
       </c>
       <c r="D143" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F143" t="inlineStr">
@@ -13951,7 +13951,7 @@
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H143" t="inlineStr">
@@ -14001,7 +14001,7 @@
       </c>
       <c r="Q143" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R143" t="inlineStr">
@@ -14601,12 +14601,12 @@
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -14616,7 +14616,7 @@
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H150" t="inlineStr">
@@ -14666,7 +14666,7 @@
       </c>
       <c r="Q150" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R150" t="inlineStr">
@@ -14696,12 +14696,12 @@
       </c>
       <c r="D151" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F151" t="inlineStr">
@@ -14711,7 +14711,7 @@
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H151" t="inlineStr">
@@ -14761,7 +14761,7 @@
       </c>
       <c r="Q151" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R151" t="inlineStr">
@@ -14791,12 +14791,12 @@
       </c>
       <c r="D152" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F152" t="inlineStr">
@@ -14806,7 +14806,7 @@
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H152" t="inlineStr">
@@ -14856,7 +14856,7 @@
       </c>
       <c r="Q152" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R152" t="inlineStr">
@@ -15646,12 +15646,12 @@
       </c>
       <c r="D161" t="inlineStr">
         <is>
-          <t>sup2</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E161" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F161" t="inlineStr">
@@ -15661,7 +15661,7 @@
       </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H161" t="inlineStr">
@@ -15711,7 +15711,7 @@
       </c>
       <c r="Q161" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R161" t="inlineStr">
@@ -16311,12 +16311,12 @@
       </c>
       <c r="D168" t="inlineStr">
         <is>
-          <t>sup2</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E168" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F168" t="inlineStr">
@@ -16326,7 +16326,7 @@
       </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H168" t="inlineStr">
@@ -16376,7 +16376,7 @@
       </c>
       <c r="Q168" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R168" t="inlineStr">
@@ -16406,12 +16406,12 @@
       </c>
       <c r="D169" t="inlineStr">
         <is>
-          <t>sup2</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E169" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F169" t="inlineStr">
@@ -16421,7 +16421,7 @@
       </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H169" t="inlineStr">
@@ -16471,7 +16471,7 @@
       </c>
       <c r="Q169" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R169" t="inlineStr">
@@ -16501,12 +16501,12 @@
       </c>
       <c r="D170" t="inlineStr">
         <is>
-          <t>sup2</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E170" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F170" t="inlineStr">
@@ -16516,7 +16516,7 @@
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H170" t="inlineStr">
@@ -16566,7 +16566,7 @@
       </c>
       <c r="Q170" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R170" t="inlineStr">
@@ -17356,12 +17356,12 @@
       </c>
       <c r="D179" t="inlineStr">
         <is>
-          <t>sup2</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E179" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F179" t="inlineStr">
@@ -17371,7 +17371,7 @@
       </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H179" t="inlineStr">
@@ -17421,7 +17421,7 @@
       </c>
       <c r="Q179" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R179" t="inlineStr">
@@ -18021,12 +18021,12 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>sup2</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E186" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F186" t="inlineStr">
@@ -18036,7 +18036,7 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H186" t="inlineStr">
@@ -18086,7 +18086,7 @@
       </c>
       <c r="Q186" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R186" t="inlineStr">
@@ -18116,12 +18116,12 @@
       </c>
       <c r="D187" t="inlineStr">
         <is>
-          <t>sup2</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E187" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F187" t="inlineStr">
@@ -18131,7 +18131,7 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H187" t="inlineStr">
@@ -18181,7 +18181,7 @@
       </c>
       <c r="Q187" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R187" t="inlineStr">
@@ -18401,12 +18401,12 @@
       </c>
       <c r="D190" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E190" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F190" t="inlineStr">
@@ -18416,7 +18416,7 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H190" t="inlineStr">
@@ -18466,7 +18466,7 @@
       </c>
       <c r="Q190" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R190" t="inlineStr">
@@ -18496,12 +18496,12 @@
       </c>
       <c r="D191" t="inlineStr">
         <is>
-          <t>hol1</t>
+          <t>sup1</t>
         </is>
       </c>
       <c r="E191" t="inlineStr">
         <is>
-          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
+          <t>root.pop_energySuppliers[0]</t>
         </is>
       </c>
       <c r="F191" t="inlineStr">
@@ -19066,12 +19066,12 @@
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E197" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F197" t="inlineStr">
@@ -19081,7 +19081,7 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H197" t="inlineStr">
@@ -19131,7 +19131,7 @@
       </c>
       <c r="Q197" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R197" t="inlineStr">
@@ -19161,12 +19161,12 @@
       </c>
       <c r="D198" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E198" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F198" t="inlineStr">
@@ -19176,7 +19176,7 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H198" t="inlineStr">
@@ -19226,7 +19226,7 @@
       </c>
       <c r="Q198" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R198" t="inlineStr">
@@ -19256,12 +19256,12 @@
       </c>
       <c r="D199" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E199" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F199" t="inlineStr">
@@ -19271,7 +19271,7 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H199" t="inlineStr">
@@ -19321,7 +19321,7 @@
       </c>
       <c r="Q199" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R199" t="inlineStr">
@@ -20111,12 +20111,12 @@
       </c>
       <c r="D208" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
@@ -20126,7 +20126,7 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H208" t="inlineStr">
@@ -20176,7 +20176,7 @@
       </c>
       <c r="Q208" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R208" t="inlineStr">
@@ -20776,12 +20776,12 @@
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E215" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F215" t="inlineStr">
@@ -20791,7 +20791,7 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H215" t="inlineStr">
@@ -20841,7 +20841,7 @@
       </c>
       <c r="Q215" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R215" t="inlineStr">
@@ -20871,12 +20871,12 @@
       </c>
       <c r="D216" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E216" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F216" t="inlineStr">
@@ -20886,7 +20886,7 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H216" t="inlineStr">
@@ -20936,7 +20936,7 @@
       </c>
       <c r="Q216" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R216" t="inlineStr">
@@ -20966,12 +20966,12 @@
       </c>
       <c r="D217" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E217" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F217" t="inlineStr">
@@ -20981,7 +20981,7 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H217" t="inlineStr">
@@ -21031,7 +21031,7 @@
       </c>
       <c r="Q217" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R217" t="inlineStr">
@@ -21821,12 +21821,12 @@
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E226" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F226" t="inlineStr">
@@ -21836,7 +21836,7 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H226" t="inlineStr">
@@ -21886,7 +21886,7 @@
       </c>
       <c r="Q226" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R226" t="inlineStr">
@@ -22486,12 +22486,12 @@
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E233" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F233" t="inlineStr">
@@ -22501,7 +22501,7 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H233" t="inlineStr">
@@ -22551,7 +22551,7 @@
       </c>
       <c r="Q233" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R233" t="inlineStr">
@@ -22581,12 +22581,12 @@
       </c>
       <c r="D234" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E234" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F234" t="inlineStr">
@@ -22596,7 +22596,7 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H234" t="inlineStr">
@@ -22646,7 +22646,7 @@
       </c>
       <c r="Q234" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R234" t="inlineStr">
@@ -22676,12 +22676,12 @@
       </c>
       <c r="D235" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E235" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F235" t="inlineStr">
@@ -22691,7 +22691,7 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H235" t="inlineStr">
@@ -22741,7 +22741,7 @@
       </c>
       <c r="Q235" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R235" t="inlineStr">
@@ -23531,12 +23531,12 @@
       </c>
       <c r="D244" t="inlineStr">
         <is>
-          <t>sup2</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E244" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F244" t="inlineStr">
@@ -23546,7 +23546,7 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H244" t="inlineStr">
@@ -23596,7 +23596,7 @@
       </c>
       <c r="Q244" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R244" t="inlineStr">
@@ -24196,12 +24196,12 @@
       </c>
       <c r="D251" t="inlineStr">
         <is>
-          <t>sup2</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E251" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F251" t="inlineStr">
@@ -24211,7 +24211,7 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H251" t="inlineStr">
@@ -24261,7 +24261,7 @@
       </c>
       <c r="Q251" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R251" t="inlineStr">
@@ -24291,12 +24291,12 @@
       </c>
       <c r="D252" t="inlineStr">
         <is>
-          <t>sup2</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E252" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F252" t="inlineStr">
@@ -24306,7 +24306,7 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H252" t="inlineStr">
@@ -24356,7 +24356,7 @@
       </c>
       <c r="Q252" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R252" t="inlineStr">
@@ -24386,12 +24386,12 @@
       </c>
       <c r="D253" t="inlineStr">
         <is>
-          <t>sup2</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E253" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F253" t="inlineStr">
@@ -24401,7 +24401,7 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H253" t="inlineStr">
@@ -24451,7 +24451,7 @@
       </c>
       <c r="Q253" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R253" t="inlineStr">
@@ -25241,12 +25241,12 @@
       </c>
       <c r="D262" t="inlineStr">
         <is>
-          <t>sup2</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E262" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F262" t="inlineStr">
@@ -25256,7 +25256,7 @@
       </c>
       <c r="G262" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H262" t="inlineStr">
@@ -25306,7 +25306,7 @@
       </c>
       <c r="Q262" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R262" t="inlineStr">
@@ -25906,12 +25906,12 @@
       </c>
       <c r="D269" t="inlineStr">
         <is>
-          <t>sup2</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F269" t="inlineStr">
@@ -25921,7 +25921,7 @@
       </c>
       <c r="G269" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H269" t="inlineStr">
@@ -25971,7 +25971,7 @@
       </c>
       <c r="Q269" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R269" t="inlineStr">
@@ -26001,12 +26001,12 @@
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>sup2</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F270" t="inlineStr">
@@ -26016,7 +26016,7 @@
       </c>
       <c r="G270" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H270" t="inlineStr">
@@ -26066,7 +26066,7 @@
       </c>
       <c r="Q270" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R270" t="inlineStr">
@@ -26096,12 +26096,12 @@
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
@@ -26111,7 +26111,7 @@
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H271" t="inlineStr">
@@ -26161,7 +26161,7 @@
       </c>
       <c r="Q271" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R271" t="inlineStr">
@@ -26381,12 +26381,12 @@
       </c>
       <c r="D274" t="inlineStr">
         <is>
-          <t>hol1</t>
+          <t>sup1</t>
         </is>
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
+          <t>root.pop_energySuppliers[0]</t>
         </is>
       </c>
       <c r="F274" t="inlineStr">
@@ -26951,12 +26951,12 @@
       </c>
       <c r="D280" t="inlineStr">
         <is>
-          <t>sup1</t>
+          <t>hol1</t>
         </is>
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[0]</t>
+          <t>root.pop_energyHolons[0]( p_actorID = hol1, p_actorType = holon, p_parentActorID = sup2 )</t>
         </is>
       </c>
       <c r="F280" t="inlineStr">
@@ -26966,7 +26966,7 @@
       </c>
       <c r="G280" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H280" t="inlineStr">
@@ -27016,7 +27016,7 @@
       </c>
       <c r="Q280" t="inlineStr">
         <is>
-          <t>-397.68946969658555</t>
+          <t>0.0</t>
         </is>
       </c>
       <c r="R280" t="inlineStr">
@@ -27536,7 +27536,7 @@
       </c>
       <c r="G286" t="inlineStr">
         <is>
-          <t>root.pop_energySuppliers[1]</t>
+          <t>null</t>
         </is>
       </c>
       <c r="H286" t="inlineStr">

</xml_diff>

<commit_message>
Fixed district heating functionality after merge
Also roughly tuned parameters of district heating system and holon-members to get some heat 'harvesting' in summer that is used in winter.
</commit_message>
<xml_diff>
--- a/Base/APIOutputAgentData_300_gridConnections.xlsx
+++ b/Base/APIOutputAgentData_300_gridConnections.xlsx
@@ -19931,7 +19931,7 @@
       </c>
       <c r="F206" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[222]</t>
+          <t>root.pop_gridConnections[221]</t>
         </is>
       </c>
       <c r="G206" t="inlineStr">
@@ -19981,7 +19981,7 @@
       </c>
       <c r="P206" t="inlineStr">
         <is>
-          <t>-382.0718635647259</t>
+          <t>-342.75986356469923</t>
         </is>
       </c>
       <c r="Q206" t="inlineStr">
@@ -20026,7 +20026,7 @@
       </c>
       <c r="F207" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[223]</t>
+          <t>root.pop_gridConnections[222]</t>
         </is>
       </c>
       <c r="G207" t="inlineStr">
@@ -20076,7 +20076,7 @@
       </c>
       <c r="P207" t="inlineStr">
         <is>
-          <t>-187.69586356462963</t>
+          <t>-382.0718635647259</t>
         </is>
       </c>
       <c r="Q207" t="inlineStr">
@@ -20121,7 +20121,7 @@
       </c>
       <c r="F208" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[224]</t>
+          <t>root.pop_gridConnections[223]</t>
         </is>
       </c>
       <c r="G208" t="inlineStr">
@@ -20171,7 +20171,7 @@
       </c>
       <c r="P208" t="inlineStr">
         <is>
-          <t>-633.2318635648804</t>
+          <t>-187.69586356462963</t>
         </is>
       </c>
       <c r="Q208" t="inlineStr">
@@ -20216,7 +20216,7 @@
       </c>
       <c r="F209" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[225]</t>
+          <t>root.pop_gridConnections[224]</t>
         </is>
       </c>
       <c r="G209" t="inlineStr">
@@ -20266,7 +20266,7 @@
       </c>
       <c r="P209" t="inlineStr">
         <is>
-          <t>-770.151863564898</t>
+          <t>-633.2318635648804</t>
         </is>
       </c>
       <c r="Q209" t="inlineStr">
@@ -20311,7 +20311,7 @@
       </c>
       <c r="F210" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[226]</t>
+          <t>root.pop_gridConnections[225]</t>
         </is>
       </c>
       <c r="G210" t="inlineStr">
@@ -20361,7 +20361,7 @@
       </c>
       <c r="P210" t="inlineStr">
         <is>
-          <t>-1039.3718635649357</t>
+          <t>-770.151863564898</t>
         </is>
       </c>
       <c r="Q210" t="inlineStr">
@@ -20406,7 +20406,7 @@
       </c>
       <c r="F211" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[227]</t>
+          <t>root.pop_gridConnections[226]</t>
         </is>
       </c>
       <c r="G211" t="inlineStr">
@@ -20456,7 +20456,7 @@
       </c>
       <c r="P211" t="inlineStr">
         <is>
-          <t>-1275.7478635649186</t>
+          <t>-1039.3718635649357</t>
         </is>
       </c>
       <c r="Q211" t="inlineStr">
@@ -20501,7 +20501,7 @@
       </c>
       <c r="F212" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[228]</t>
+          <t>root.pop_gridConnections[227]</t>
         </is>
       </c>
       <c r="G212" t="inlineStr">
@@ -20551,7 +20551,7 @@
       </c>
       <c r="P212" t="inlineStr">
         <is>
-          <t>-439.19186356476405</t>
+          <t>-1275.7478635649186</t>
         </is>
       </c>
       <c r="Q212" t="inlineStr">
@@ -20596,7 +20596,7 @@
       </c>
       <c r="F213" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[229]</t>
+          <t>root.pop_gridConnections[228]</t>
         </is>
       </c>
       <c r="G213" t="inlineStr">
@@ -20646,7 +20646,7 @@
       </c>
       <c r="P213" t="inlineStr">
         <is>
-          <t>-266.3198635646405</t>
+          <t>-439.19186356476405</t>
         </is>
       </c>
       <c r="Q213" t="inlineStr">
@@ -20691,7 +20691,7 @@
       </c>
       <c r="F214" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[230]</t>
+          <t>root.pop_gridConnections[229]</t>
         </is>
       </c>
       <c r="G214" t="inlineStr">
@@ -20741,7 +20741,7 @@
       </c>
       <c r="P214" t="inlineStr">
         <is>
-          <t>-277.23986356464917</t>
+          <t>-266.3198635646405</t>
         </is>
       </c>
       <c r="Q214" t="inlineStr">
@@ -20786,7 +20786,7 @@
       </c>
       <c r="F215" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[231]</t>
+          <t>root.pop_gridConnections[230]</t>
         </is>
       </c>
       <c r="G215" t="inlineStr">
@@ -20836,7 +20836,7 @@
       </c>
       <c r="P215" t="inlineStr">
         <is>
-          <t>-280.3058635646509</t>
+          <t>-277.23986356464917</t>
         </is>
       </c>
       <c r="Q215" t="inlineStr">
@@ -20881,7 +20881,7 @@
       </c>
       <c r="F216" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[232]</t>
+          <t>root.pop_gridConnections[231]</t>
         </is>
       </c>
       <c r="G216" t="inlineStr">
@@ -20931,7 +20931,7 @@
       </c>
       <c r="P216" t="inlineStr">
         <is>
-          <t>-379.8878635647259</t>
+          <t>-280.3058635646509</t>
         </is>
       </c>
       <c r="Q216" t="inlineStr">
@@ -20976,7 +20976,7 @@
       </c>
       <c r="F217" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[233]</t>
+          <t>root.pop_gridConnections[232]</t>
         </is>
       </c>
       <c r="G217" t="inlineStr">
@@ -21026,7 +21026,7 @@
       </c>
       <c r="P217" t="inlineStr">
         <is>
-          <t>-663.6398635648867</t>
+          <t>-379.8878635647259</t>
         </is>
       </c>
       <c r="Q217" t="inlineStr">
@@ -21071,7 +21071,7 @@
       </c>
       <c r="F218" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[234]</t>
+          <t>root.pop_gridConnections[233]</t>
         </is>
       </c>
       <c r="G218" t="inlineStr">
@@ -21121,7 +21121,7 @@
       </c>
       <c r="P218" t="inlineStr">
         <is>
-          <t>-168.0398635646302</t>
+          <t>-663.6398635648867</t>
         </is>
       </c>
       <c r="Q218" t="inlineStr">
@@ -21166,7 +21166,7 @@
       </c>
       <c r="F219" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[235]</t>
+          <t>root.pop_gridConnections[234]</t>
         </is>
       </c>
       <c r="G219" t="inlineStr">
@@ -21216,7 +21216,7 @@
       </c>
       <c r="P219" t="inlineStr">
         <is>
-          <t>-139.64786356463966</t>
+          <t>-168.0398635646302</t>
         </is>
       </c>
       <c r="Q219" t="inlineStr">
@@ -21261,7 +21261,7 @@
       </c>
       <c r="F220" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[236]</t>
+          <t>root.pop_gridConnections[235]</t>
         </is>
       </c>
       <c r="G220" t="inlineStr">
@@ -21311,7 +21311,7 @@
       </c>
       <c r="P220" t="inlineStr">
         <is>
-          <t>-287.73986356465736</t>
+          <t>-139.64786356463966</t>
         </is>
       </c>
       <c r="Q220" t="inlineStr">
@@ -21356,7 +21356,7 @@
       </c>
       <c r="F221" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[237]</t>
+          <t>root.pop_gridConnections[236]</t>
         </is>
       </c>
       <c r="G221" t="inlineStr">
@@ -21406,7 +21406,7 @@
       </c>
       <c r="P221" t="inlineStr">
         <is>
-          <t>-518.9918635648086</t>
+          <t>-287.73986356465736</t>
         </is>
       </c>
       <c r="Q221" t="inlineStr">
@@ -21451,7 +21451,7 @@
       </c>
       <c r="F222" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[238]</t>
+          <t>root.pop_gridConnections[237]</t>
         </is>
       </c>
       <c r="G222" t="inlineStr">
@@ -21501,7 +21501,7 @@
       </c>
       <c r="P222" t="inlineStr">
         <is>
-          <t>-395.1758635647387</t>
+          <t>-518.9918635648086</t>
         </is>
       </c>
       <c r="Q222" t="inlineStr">
@@ -21546,7 +21546,7 @@
       </c>
       <c r="F223" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[239]</t>
+          <t>root.pop_gridConnections[238]</t>
         </is>
       </c>
       <c r="G223" t="inlineStr">
@@ -21596,7 +21596,7 @@
       </c>
       <c r="P223" t="inlineStr">
         <is>
-          <t>-255.3998635646296</t>
+          <t>-395.1758635647387</t>
         </is>
       </c>
       <c r="Q223" t="inlineStr">
@@ -21641,7 +21641,7 @@
       </c>
       <c r="F224" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[240]</t>
+          <t>root.pop_gridConnections[239]</t>
         </is>
       </c>
       <c r="G224" t="inlineStr">
@@ -21691,7 +21691,7 @@
       </c>
       <c r="P224" t="inlineStr">
         <is>
-          <t>-880.0238635649142</t>
+          <t>-255.3998635646296</t>
         </is>
       </c>
       <c r="Q224" t="inlineStr">
@@ -21736,7 +21736,7 @@
       </c>
       <c r="F225" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[241]</t>
+          <t>root.pop_gridConnections[240]</t>
         </is>
       </c>
       <c r="G225" t="inlineStr">
@@ -21786,7 +21786,7 @@
       </c>
       <c r="P225" t="inlineStr">
         <is>
-          <t>-746.2538635648955</t>
+          <t>-880.0238635649142</t>
         </is>
       </c>
       <c r="Q225" t="inlineStr">
@@ -21831,7 +21831,7 @@
       </c>
       <c r="F226" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[242]</t>
+          <t>root.pop_gridConnections[241]</t>
         </is>
       </c>
       <c r="G226" t="inlineStr">
@@ -21881,7 +21881,7 @@
       </c>
       <c r="P226" t="inlineStr">
         <is>
-          <t>-135.27986356464095</t>
+          <t>-746.2538635648955</t>
         </is>
       </c>
       <c r="Q226" t="inlineStr">
@@ -21926,7 +21926,7 @@
       </c>
       <c r="F227" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[243]</t>
+          <t>root.pop_gridConnections[242]</t>
         </is>
       </c>
       <c r="G227" t="inlineStr">
@@ -21976,7 +21976,7 @@
       </c>
       <c r="P227" t="inlineStr">
         <is>
-          <t>-2929.8758635647346</t>
+          <t>-135.27986356464095</t>
         </is>
       </c>
       <c r="Q227" t="inlineStr">
@@ -22021,7 +22021,7 @@
       </c>
       <c r="F228" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[244]</t>
+          <t>root.pop_gridConnections[243]</t>
         </is>
       </c>
       <c r="G228" t="inlineStr">
@@ -22071,7 +22071,7 @@
       </c>
       <c r="P228" t="inlineStr">
         <is>
-          <t>-2013.939863564789</t>
+          <t>-2929.8758635647346</t>
         </is>
       </c>
       <c r="Q228" t="inlineStr">
@@ -22116,7 +22116,7 @@
       </c>
       <c r="F229" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[245]</t>
+          <t>root.pop_gridConnections[244]</t>
         </is>
       </c>
       <c r="G229" t="inlineStr">
@@ -22166,7 +22166,7 @@
       </c>
       <c r="P229" t="inlineStr">
         <is>
-          <t>-268.7978635646423</t>
+          <t>-2013.939863564789</t>
         </is>
       </c>
       <c r="Q229" t="inlineStr">
@@ -22211,7 +22211,7 @@
       </c>
       <c r="F230" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[246]</t>
+          <t>root.pop_gridConnections[245]</t>
         </is>
       </c>
       <c r="G230" t="inlineStr">
@@ -22261,7 +22261,7 @@
       </c>
       <c r="P230" t="inlineStr">
         <is>
-          <t>-950.2478635649197</t>
+          <t>-268.7978635646423</t>
         </is>
       </c>
       <c r="Q230" t="inlineStr">
@@ -22306,7 +22306,7 @@
       </c>
       <c r="F231" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[247]</t>
+          <t>root.pop_gridConnections[246]</t>
         </is>
       </c>
       <c r="G231" t="inlineStr">
@@ -22356,7 +22356,7 @@
       </c>
       <c r="P231" t="inlineStr">
         <is>
-          <t>-353.6798635647065</t>
+          <t>-950.2478635649197</t>
         </is>
       </c>
       <c r="Q231" t="inlineStr">
@@ -22401,7 +22401,7 @@
       </c>
       <c r="F232" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[248]</t>
+          <t>root.pop_gridConnections[247]</t>
         </is>
       </c>
       <c r="G232" t="inlineStr">
@@ -22451,7 +22451,7 @@
       </c>
       <c r="P232" t="inlineStr">
         <is>
-          <t>-246.0758635646293</t>
+          <t>-353.6798635647065</t>
         </is>
       </c>
       <c r="Q232" t="inlineStr">
@@ -22496,7 +22496,7 @@
       </c>
       <c r="F233" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[249]</t>
+          <t>root.pop_gridConnections[248]</t>
         </is>
       </c>
       <c r="G233" t="inlineStr">
@@ -22546,7 +22546,7 @@
       </c>
       <c r="P233" t="inlineStr">
         <is>
-          <t>-413.1938635647472</t>
+          <t>-246.0758635646293</t>
         </is>
       </c>
       <c r="Q233" t="inlineStr">
@@ -22591,7 +22591,7 @@
       </c>
       <c r="F234" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[250]</t>
+          <t>root.pop_gridConnections[249]</t>
         </is>
       </c>
       <c r="G234" t="inlineStr">
@@ -22641,7 +22641,7 @@
       </c>
       <c r="P234" t="inlineStr">
         <is>
-          <t>-372.2438635647198</t>
+          <t>-413.1938635647472</t>
         </is>
       </c>
       <c r="Q234" t="inlineStr">
@@ -22686,7 +22686,7 @@
       </c>
       <c r="F235" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[251]</t>
+          <t>root.pop_gridConnections[250]</t>
         </is>
       </c>
       <c r="G235" t="inlineStr">
@@ -22736,7 +22736,7 @@
       </c>
       <c r="P235" t="inlineStr">
         <is>
-          <t>-327.26186356468696</t>
+          <t>-372.2438635647198</t>
         </is>
       </c>
       <c r="Q235" t="inlineStr">
@@ -22781,7 +22781,7 @@
       </c>
       <c r="F236" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[252]</t>
+          <t>root.pop_gridConnections[251]</t>
         </is>
       </c>
       <c r="G236" t="inlineStr">
@@ -22831,7 +22831,7 @@
       </c>
       <c r="P236" t="inlineStr">
         <is>
-          <t>-368.96786356471677</t>
+          <t>-327.26186356468696</t>
         </is>
       </c>
       <c r="Q236" t="inlineStr">
@@ -22876,7 +22876,7 @@
       </c>
       <c r="F237" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[253]</t>
+          <t>root.pop_gridConnections[252]</t>
         </is>
       </c>
       <c r="G237" t="inlineStr">
@@ -22926,7 +22926,7 @@
       </c>
       <c r="P237" t="inlineStr">
         <is>
-          <t>-414.4958635647474</t>
+          <t>-368.96786356471677</t>
         </is>
       </c>
       <c r="Q237" t="inlineStr">
@@ -22971,7 +22971,7 @@
       </c>
       <c r="F238" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[254]</t>
+          <t>root.pop_gridConnections[253]</t>
         </is>
       </c>
       <c r="G238" t="inlineStr">
@@ -23021,7 +23021,7 @@
       </c>
       <c r="P238" t="inlineStr">
         <is>
-          <t>-185.51186356462998</t>
+          <t>-414.4958635647474</t>
         </is>
       </c>
       <c r="Q238" t="inlineStr">
@@ -23066,7 +23066,7 @@
       </c>
       <c r="F239" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[255]</t>
+          <t>root.pop_gridConnections[254]</t>
         </is>
       </c>
       <c r="G239" t="inlineStr">
@@ -23116,7 +23116,7 @@
       </c>
       <c r="P239" t="inlineStr">
         <is>
-          <t>-417.477863564753</t>
+          <t>-185.51186356462998</t>
         </is>
       </c>
       <c r="Q239" t="inlineStr">
@@ -23161,7 +23161,7 @@
       </c>
       <c r="F240" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[256]</t>
+          <t>root.pop_gridConnections[255]</t>
         </is>
       </c>
       <c r="G240" t="inlineStr">
@@ -23211,7 +23211,7 @@
       </c>
       <c r="P240" t="inlineStr">
         <is>
-          <t>-2524.9958635647026</t>
+          <t>-417.477863564753</t>
         </is>
       </c>
       <c r="Q240" t="inlineStr">
@@ -23256,7 +23256,7 @@
       </c>
       <c r="F241" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[257]</t>
+          <t>root.pop_gridConnections[256]</t>
         </is>
       </c>
       <c r="G241" t="inlineStr">
@@ -23306,7 +23306,7 @@
       </c>
       <c r="P241" t="inlineStr">
         <is>
-          <t>-209.5358635646299</t>
+          <t>-2524.9958635647026</t>
         </is>
       </c>
       <c r="Q241" t="inlineStr">
@@ -23351,7 +23351,7 @@
       </c>
       <c r="F242" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[258]</t>
+          <t>root.pop_gridConnections[257]</t>
         </is>
       </c>
       <c r="G242" t="inlineStr">
@@ -23401,7 +23401,7 @@
       </c>
       <c r="P242" t="inlineStr">
         <is>
-          <t>-152.7518635646358</t>
+          <t>-209.5358635646299</t>
         </is>
       </c>
       <c r="Q242" t="inlineStr">
@@ -23446,7 +23446,7 @@
       </c>
       <c r="F243" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[259]</t>
+          <t>root.pop_gridConnections[258]</t>
         </is>
       </c>
       <c r="G243" t="inlineStr">
@@ -23496,7 +23496,7 @@
       </c>
       <c r="P243" t="inlineStr">
         <is>
-          <t>-234.14786356462955</t>
+          <t>-152.7518635646358</t>
         </is>
       </c>
       <c r="Q243" t="inlineStr">
@@ -23541,7 +23541,7 @@
       </c>
       <c r="F244" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[260]</t>
+          <t>root.pop_gridConnections[259]</t>
         </is>
       </c>
       <c r="G244" t="inlineStr">
@@ -23591,7 +23591,7 @@
       </c>
       <c r="P244" t="inlineStr">
         <is>
-          <t>-490.1798635647937</t>
+          <t>-234.14786356462955</t>
         </is>
       </c>
       <c r="Q244" t="inlineStr">
@@ -23636,7 +23636,7 @@
       </c>
       <c r="F245" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[261]</t>
+          <t>root.pop_gridConnections[260]</t>
         </is>
       </c>
       <c r="G245" t="inlineStr">
@@ -23686,7 +23686,7 @@
       </c>
       <c r="P245" t="inlineStr">
         <is>
-          <t>-202.98386356463016</t>
+          <t>-490.1798635647937</t>
         </is>
       </c>
       <c r="Q245" t="inlineStr">
@@ -23731,7 +23731,7 @@
       </c>
       <c r="F246" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[262]</t>
+          <t>root.pop_gridConnections[261]</t>
         </is>
       </c>
       <c r="G246" t="inlineStr">
@@ -23781,7 +23781,7 @@
       </c>
       <c r="P246" t="inlineStr">
         <is>
-          <t>-644.9078635648843</t>
+          <t>-202.98386356463016</t>
         </is>
       </c>
       <c r="Q246" t="inlineStr">
@@ -23826,7 +23826,7 @@
       </c>
       <c r="F247" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[263]</t>
+          <t>root.pop_gridConnections[262]</t>
         </is>
       </c>
       <c r="G247" t="inlineStr">
@@ -23876,7 +23876,7 @@
       </c>
       <c r="P247" t="inlineStr">
         <is>
-          <t>-401.7278635647412</t>
+          <t>-644.9078635648843</t>
         </is>
       </c>
       <c r="Q247" t="inlineStr">
@@ -23921,7 +23921,7 @@
       </c>
       <c r="F248" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[264]</t>
+          <t>root.pop_gridConnections[263]</t>
         </is>
       </c>
       <c r="G248" t="inlineStr">
@@ -23971,7 +23971,7 @@
       </c>
       <c r="P248" t="inlineStr">
         <is>
-          <t>-164.2178635646303</t>
+          <t>-401.7278635647412</t>
         </is>
       </c>
       <c r="Q248" t="inlineStr">
@@ -24016,7 +24016,7 @@
       </c>
       <c r="F249" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[265]</t>
+          <t>root.pop_gridConnections[264]</t>
         </is>
       </c>
       <c r="G249" t="inlineStr">
@@ -24066,7 +24066,7 @@
       </c>
       <c r="P249" t="inlineStr">
         <is>
-          <t>-547.7198635648267</t>
+          <t>-164.2178635646303</t>
         </is>
       </c>
       <c r="Q249" t="inlineStr">
@@ -24111,7 +24111,7 @@
       </c>
       <c r="F250" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[266]</t>
+          <t>root.pop_gridConnections[265]</t>
         </is>
       </c>
       <c r="G250" t="inlineStr">
@@ -24161,7 +24161,7 @@
       </c>
       <c r="P250" t="inlineStr">
         <is>
-          <t>-146.19986356463835</t>
+          <t>-547.7198635648267</t>
         </is>
       </c>
       <c r="Q250" t="inlineStr">
@@ -24206,7 +24206,7 @@
       </c>
       <c r="F251" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[267]</t>
+          <t>root.pop_gridConnections[266]</t>
         </is>
       </c>
       <c r="G251" t="inlineStr">
@@ -24256,7 +24256,7 @@
       </c>
       <c r="P251" t="inlineStr">
         <is>
-          <t>-272.87186356464616</t>
+          <t>-146.19986356463835</t>
         </is>
       </c>
       <c r="Q251" t="inlineStr">
@@ -24301,7 +24301,7 @@
       </c>
       <c r="F252" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[268]</t>
+          <t>root.pop_gridConnections[267]</t>
         </is>
       </c>
       <c r="G252" t="inlineStr">
@@ -24351,7 +24351,7 @@
       </c>
       <c r="P252" t="inlineStr">
         <is>
-          <t>-240.11186356462983</t>
+          <t>-272.87186356464616</t>
         </is>
       </c>
       <c r="Q252" t="inlineStr">
@@ -24396,7 +24396,7 @@
       </c>
       <c r="F253" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[269]</t>
+          <t>root.pop_gridConnections[268]</t>
         </is>
       </c>
       <c r="G253" t="inlineStr">
@@ -24446,7 +24446,7 @@
       </c>
       <c r="P253" t="inlineStr">
         <is>
-          <t>-237.92786356462935</t>
+          <t>-240.11186356462983</t>
         </is>
       </c>
       <c r="Q253" t="inlineStr">
@@ -24491,7 +24491,7 @@
       </c>
       <c r="F254" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[270]</t>
+          <t>root.pop_gridConnections[269]</t>
         </is>
       </c>
       <c r="G254" t="inlineStr">
@@ -24541,7 +24541,7 @@
       </c>
       <c r="P254" t="inlineStr">
         <is>
-          <t>-266.31986356463926</t>
+          <t>-237.92786356462935</t>
         </is>
       </c>
       <c r="Q254" t="inlineStr">
@@ -24586,7 +24586,7 @@
       </c>
       <c r="F255" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[271]</t>
+          <t>root.pop_gridConnections[270]</t>
         </is>
       </c>
       <c r="G255" t="inlineStr">
@@ -24636,7 +24636,7 @@
       </c>
       <c r="P255" t="inlineStr">
         <is>
-          <t>-403.91186356474157</t>
+          <t>-266.31986356463926</t>
         </is>
       </c>
       <c r="Q255" t="inlineStr">
@@ -24681,7 +24681,7 @@
       </c>
       <c r="F256" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[272]</t>
+          <t>root.pop_gridConnections[271]</t>
         </is>
       </c>
       <c r="G256" t="inlineStr">
@@ -24731,7 +24731,7 @@
       </c>
       <c r="P256" t="inlineStr">
         <is>
-          <t>-198.61586356462976</t>
+          <t>-403.91186356474157</t>
         </is>
       </c>
       <c r="Q256" t="inlineStr">
@@ -24776,7 +24776,7 @@
       </c>
       <c r="F257" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[273]</t>
+          <t>root.pop_gridConnections[272]</t>
         </is>
       </c>
       <c r="G257" t="inlineStr">
@@ -24826,7 +24826,7 @@
       </c>
       <c r="P257" t="inlineStr">
         <is>
-          <t>-711.8558635648923</t>
+          <t>-198.61586356462976</t>
         </is>
       </c>
       <c r="Q257" t="inlineStr">
@@ -24871,7 +24871,7 @@
       </c>
       <c r="F258" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[274]</t>
+          <t>root.pop_gridConnections[273]</t>
         </is>
       </c>
       <c r="G258" t="inlineStr">
@@ -24921,7 +24921,7 @@
       </c>
       <c r="P258" t="inlineStr">
         <is>
-          <t>-340.5758635646977</t>
+          <t>-711.8558635648923</t>
         </is>
       </c>
       <c r="Q258" t="inlineStr">
@@ -24966,7 +24966,7 @@
       </c>
       <c r="F259" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[275]</t>
+          <t>root.pop_gridConnections[274]</t>
         </is>
       </c>
       <c r="G259" t="inlineStr">
@@ -25016,7 +25016,7 @@
       </c>
       <c r="P259" t="inlineStr">
         <is>
-          <t>-545.4518635648261</t>
+          <t>-340.5758635646977</t>
         </is>
       </c>
       <c r="Q259" t="inlineStr">
@@ -25061,7 +25061,7 @@
       </c>
       <c r="F260" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[276]</t>
+          <t>root.pop_gridConnections[275]</t>
         </is>
       </c>
       <c r="G260" t="inlineStr">
@@ -25111,7 +25111,7 @@
       </c>
       <c r="P260" t="inlineStr">
         <is>
-          <t>-622.6478635648753</t>
+          <t>-545.4518635648261</t>
         </is>
       </c>
       <c r="Q260" t="inlineStr">
@@ -25156,7 +25156,7 @@
       </c>
       <c r="F261" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[277]</t>
+          <t>root.pop_gridConnections[276]</t>
         </is>
       </c>
       <c r="G261" t="inlineStr">
@@ -25206,7 +25206,7 @@
       </c>
       <c r="P261" t="inlineStr">
         <is>
-          <t>-824.6678635649091</t>
+          <t>-622.6478635648753</t>
         </is>
       </c>
       <c r="Q261" t="inlineStr">
@@ -25251,7 +25251,7 @@
       </c>
       <c r="F262" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[278]</t>
+          <t>root.pop_gridConnections[277]</t>
         </is>
       </c>
       <c r="G262" t="inlineStr">
@@ -25301,7 +25301,7 @@
       </c>
       <c r="P262" t="inlineStr">
         <is>
-          <t>-707.4458635648913</t>
+          <t>-824.6678635649091</t>
         </is>
       </c>
       <c r="Q262" t="inlineStr">
@@ -25346,7 +25346,7 @@
       </c>
       <c r="F263" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[279]</t>
+          <t>root.pop_gridConnections[278]</t>
         </is>
       </c>
       <c r="G263" t="inlineStr">
@@ -25396,7 +25396,7 @@
       </c>
       <c r="P263" t="inlineStr">
         <is>
-          <t>-320.9198635646831</t>
+          <t>-707.4458635648913</t>
         </is>
       </c>
       <c r="Q263" t="inlineStr">
@@ -25441,7 +25441,7 @@
       </c>
       <c r="F264" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[280]</t>
+          <t>root.pop_gridConnections[279]</t>
         </is>
       </c>
       <c r="G264" t="inlineStr">
@@ -25491,7 +25491,7 @@
       </c>
       <c r="P264" t="inlineStr">
         <is>
-          <t>-1344.7958635649081</t>
+          <t>-320.9198635646831</t>
         </is>
       </c>
       <c r="Q264" t="inlineStr">
@@ -25536,7 +25536,7 @@
       </c>
       <c r="F265" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[281]</t>
+          <t>root.pop_gridConnections[280]</t>
         </is>
       </c>
       <c r="G265" t="inlineStr">
@@ -25586,7 +25586,7 @@
       </c>
       <c r="P265" t="inlineStr">
         <is>
-          <t>-462.41786356477627</t>
+          <t>-1344.7958635649081</t>
         </is>
       </c>
       <c r="Q265" t="inlineStr">
@@ -25631,7 +25631,7 @@
       </c>
       <c r="F266" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[282]</t>
+          <t>root.pop_gridConnections[281]</t>
         </is>
       </c>
       <c r="G266" t="inlineStr">
@@ -25681,7 +25681,7 @@
       </c>
       <c r="P266" t="inlineStr">
         <is>
-          <t>-667.7138635648847</t>
+          <t>-462.41786356477627</t>
         </is>
       </c>
       <c r="Q266" t="inlineStr">
@@ -25726,7 +25726,7 @@
       </c>
       <c r="F267" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[283]</t>
+          <t>root.pop_gridConnections[282]</t>
         </is>
       </c>
       <c r="G267" t="inlineStr">
@@ -25776,7 +25776,7 @@
       </c>
       <c r="P267" t="inlineStr">
         <is>
-          <t>-459.0578635647758</t>
+          <t>-667.7138635648847</t>
         </is>
       </c>
       <c r="Q267" t="inlineStr">
@@ -25821,7 +25821,7 @@
       </c>
       <c r="F268" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[284]</t>
+          <t>root.pop_gridConnections[283]</t>
         </is>
       </c>
       <c r="G268" t="inlineStr">
@@ -25871,7 +25871,7 @@
       </c>
       <c r="P268" t="inlineStr">
         <is>
-          <t>-130.91186356464146</t>
+          <t>-459.0578635647758</t>
         </is>
       </c>
       <c r="Q268" t="inlineStr">
@@ -25916,7 +25916,7 @@
       </c>
       <c r="F269" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[285]</t>
+          <t>root.pop_gridConnections[284]</t>
         </is>
       </c>
       <c r="G269" t="inlineStr">
@@ -25966,7 +25966,7 @@
       </c>
       <c r="P269" t="inlineStr">
         <is>
-          <t>-508.9118635648058</t>
+          <t>-130.91186356464146</t>
         </is>
       </c>
       <c r="Q269" t="inlineStr">
@@ -26011,7 +26011,7 @@
       </c>
       <c r="F270" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[286]</t>
+          <t>root.pop_gridConnections[285]</t>
         </is>
       </c>
       <c r="G270" t="inlineStr">
@@ -26061,7 +26061,7 @@
       </c>
       <c r="P270" t="inlineStr">
         <is>
-          <t>-695.6018635648871</t>
+          <t>-508.9118635648058</t>
         </is>
       </c>
       <c r="Q270" t="inlineStr">
@@ -26106,7 +26106,7 @@
       </c>
       <c r="F271" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[287]</t>
+          <t>root.pop_gridConnections[286]</t>
         </is>
       </c>
       <c r="G271" t="inlineStr">
@@ -26156,7 +26156,7 @@
       </c>
       <c r="P271" t="inlineStr">
         <is>
-          <t>-850.9598635649144</t>
+          <t>-695.6018635648871</t>
         </is>
       </c>
       <c r="Q271" t="inlineStr">
@@ -26201,7 +26201,7 @@
       </c>
       <c r="F272" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[288]</t>
+          <t>root.pop_gridConnections[287]</t>
         </is>
       </c>
       <c r="G272" t="inlineStr">
@@ -26251,7 +26251,7 @@
       </c>
       <c r="P272" t="inlineStr">
         <is>
-          <t>-1098.4238635649417</t>
+          <t>-850.9598635649144</t>
         </is>
       </c>
       <c r="Q272" t="inlineStr">
@@ -26296,7 +26296,7 @@
       </c>
       <c r="F273" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[289]</t>
+          <t>root.pop_gridConnections[288]</t>
         </is>
       </c>
       <c r="G273" t="inlineStr">
@@ -26346,7 +26346,7 @@
       </c>
       <c r="P273" t="inlineStr">
         <is>
-          <t>-1137.1898635649397</t>
+          <t>-1098.4238635649417</t>
         </is>
       </c>
       <c r="Q273" t="inlineStr">
@@ -26391,7 +26391,7 @@
       </c>
       <c r="F274" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[290]</t>
+          <t>root.pop_gridConnections[289]</t>
         </is>
       </c>
       <c r="G274" t="inlineStr">
@@ -26441,7 +26441,7 @@
       </c>
       <c r="P274" t="inlineStr">
         <is>
-          <t>-137.46386356464026</t>
+          <t>-1137.1898635649397</t>
         </is>
       </c>
       <c r="Q274" t="inlineStr">
@@ -26486,7 +26486,7 @@
       </c>
       <c r="F275" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[291]</t>
+          <t>root.pop_gridConnections[290]</t>
         </is>
       </c>
       <c r="G275" t="inlineStr">
@@ -26536,7 +26536,7 @@
       </c>
       <c r="P275" t="inlineStr">
         <is>
-          <t>-478.1678635647865</t>
+          <t>-137.46386356464026</t>
         </is>
       </c>
       <c r="Q275" t="inlineStr">
@@ -26581,7 +26581,7 @@
       </c>
       <c r="F276" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[292]</t>
+          <t>root.pop_gridConnections[291]</t>
         </is>
       </c>
       <c r="G276" t="inlineStr">
@@ -26631,7 +26631,7 @@
       </c>
       <c r="P276" t="inlineStr">
         <is>
-          <t>-452.54786356476984</t>
+          <t>-478.1678635647865</t>
         </is>
       </c>
       <c r="Q276" t="inlineStr">
@@ -26676,7 +26676,7 @@
       </c>
       <c r="F277" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[293]</t>
+          <t>root.pop_gridConnections[292]</t>
         </is>
       </c>
       <c r="G277" t="inlineStr">
@@ -26726,7 +26726,7 @@
       </c>
       <c r="P277" t="inlineStr">
         <is>
-          <t>-216.08786356462943</t>
+          <t>-452.54786356476984</t>
         </is>
       </c>
       <c r="Q277" t="inlineStr">
@@ -26771,7 +26771,7 @@
       </c>
       <c r="F278" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[294]</t>
+          <t>root.pop_gridConnections[293]</t>
         </is>
       </c>
       <c r="G278" t="inlineStr">
@@ -26821,7 +26821,7 @@
       </c>
       <c r="P278" t="inlineStr">
         <is>
-          <t>-269.133863564642</t>
+          <t>-216.08786356462943</t>
         </is>
       </c>
       <c r="Q278" t="inlineStr">
@@ -26866,7 +26866,7 @@
       </c>
       <c r="F279" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[295]</t>
+          <t>root.pop_gridConnections[294]</t>
         </is>
       </c>
       <c r="G279" t="inlineStr">
@@ -26916,7 +26916,7 @@
       </c>
       <c r="P279" t="inlineStr">
         <is>
-          <t>-817.1918635649076</t>
+          <t>-269.133863564642</t>
         </is>
       </c>
       <c r="Q279" t="inlineStr">
@@ -26961,7 +26961,7 @@
       </c>
       <c r="F280" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[296]</t>
+          <t>root.pop_gridConnections[295]</t>
         </is>
       </c>
       <c r="G280" t="inlineStr">
@@ -27011,7 +27011,7 @@
       </c>
       <c r="P280" t="inlineStr">
         <is>
-          <t>-240.11186356462963</t>
+          <t>-817.1918635649076</t>
         </is>
       </c>
       <c r="Q280" t="inlineStr">
@@ -27056,7 +27056,7 @@
       </c>
       <c r="F281" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[297]</t>
+          <t>root.pop_gridConnections[296]</t>
         </is>
       </c>
       <c r="G281" t="inlineStr">
@@ -27106,7 +27106,7 @@
       </c>
       <c r="P281" t="inlineStr">
         <is>
-          <t>-209.87186356462982</t>
+          <t>-240.11186356462963</t>
         </is>
       </c>
       <c r="Q281" t="inlineStr">
@@ -27151,7 +27151,7 @@
       </c>
       <c r="F282" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[298]</t>
+          <t>root.pop_gridConnections[297]</t>
         </is>
       </c>
       <c r="G282" t="inlineStr">
@@ -27201,7 +27201,7 @@
       </c>
       <c r="P282" t="inlineStr">
         <is>
-          <t>-185.51186356462998</t>
+          <t>-209.87186356462982</t>
         </is>
       </c>
       <c r="Q282" t="inlineStr">
@@ -27246,7 +27246,7 @@
       </c>
       <c r="F283" t="inlineStr">
         <is>
-          <t>root.pop_gridConnections[299]</t>
+          <t>root.pop_gridConnections[298]</t>
         </is>
       </c>
       <c r="G283" t="inlineStr">
@@ -27296,7 +27296,7 @@
       </c>
       <c r="P283" t="inlineStr">
         <is>
-          <t>-670.9478635648841</t>
+          <t>-185.51186356462998</t>
         </is>
       </c>
       <c r="Q283" t="inlineStr">

</xml_diff>